<commit_message>
TB 2.5 - 2.8 Tamil 07/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C5C177-B117-4C31-9DEC-ACAEFC6431F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88578907-077D-4CC2-845E-63085458F128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5709" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5701" uniqueCount="1226">
   <si>
     <t>PS</t>
   </si>
@@ -4447,10 +4447,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1475" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1137" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1208" sqref="V1208"/>
+      <selection pane="bottomLeft" activeCell="N1156" sqref="N1156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1.1 Ghanam files pushed 20/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88578907-077D-4CC2-845E-63085458F128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5C79F5-52E0-4912-B7BA-07C13B2E7B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4448,9 +4448,9 @@
   <dimension ref="A1:W1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1137" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1156" sqref="N1156"/>
+      <selection pane="bottomLeft" activeCell="O188" sqref="O188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1 Ghanam files 22/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5C79F5-52E0-4912-B7BA-07C13B2E7B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB131098-F3C9-4794-923A-7970034C1F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3712,7 +3712,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3883,8 +3883,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3906,6 +3913,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3937,7 +3950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4163,6 +4176,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4448,9 +4464,9 @@
   <dimension ref="A1:W1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1361" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O188" sqref="O188"/>
+      <selection pane="bottomLeft" activeCell="P1370" sqref="P1370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -56851,7 +56867,7 @@
         <f t="shared" si="64"/>
         <v>61</v>
       </c>
-      <c r="N1369" s="25" t="s">
+      <c r="N1369" s="83" t="s">
         <v>218</v>
       </c>
       <c r="O1369" s="8"/>
@@ -56894,7 +56910,7 @@
         <f t="shared" si="64"/>
         <v>62</v>
       </c>
-      <c r="N1370" s="25" t="s">
+      <c r="N1370" s="83" t="s">
         <v>327</v>
       </c>
       <c r="O1370" s="8"/>

</xml_diff>

<commit_message>
TS 1.5 Ghanam inputs from Raja
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB131098-F3C9-4794-923A-7970034C1F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CEF592-24BD-4776-A2C1-F63CD6FFE229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -4463,10 +4470,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1361" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="P1370" sqref="P1370"/>
+      <selection pane="bottomLeft" activeCell="S1365" sqref="S1365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
latest Ghanam templates 09/12/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CEF592-24BD-4776-A2C1-F63CD6FFE229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C841123B-BE1B-4D45-8A3C-8FF2BF6B84EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4470,10 +4470,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1361" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S1365" sqref="S1365"/>
+      <selection pane="bottomLeft" activeCell="V1530" sqref="V1530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update to Padam Input templates 17/12/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C841123B-BE1B-4D45-8A3C-8FF2BF6B84EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40FA897-15F5-4B8E-A47C-A15836BEEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4470,10 +4470,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1530" sqref="V1530"/>
+      <selection pane="bottomLeft" activeCell="N1372" sqref="N1372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1.6 Padam Input template pushed 16/01/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40FA897-15F5-4B8E-A47C-A15836BEEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E081D5D2-9DCF-40C7-A385-AB2364AF588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3719,19 +3719,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3957,235 +3951,232 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4470,10 +4461,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1372" sqref="N1372"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5003,7 +4994,7 @@
       <c r="U1" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="V1" s="73" t="s">
+      <c r="V1" s="14" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6902,7 +6893,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N48" s="75" t="s">
+      <c r="N48" s="74" t="s">
         <v>290</v>
       </c>
       <c r="O48" s="9" t="s">
@@ -7983,7 +7974,7 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N75" s="79" t="s">
+      <c r="N75" s="78" t="s">
         <v>395</v>
       </c>
       <c r="O75" s="9" t="s">
@@ -8608,7 +8599,7 @@
         <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="N91" s="80" t="s">
+      <c r="N91" s="79" t="s">
         <v>1222</v>
       </c>
       <c r="O91" s="9" t="s">
@@ -11746,7 +11737,7 @@
       <c r="N173" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="O173" s="81" t="s">
+      <c r="O173" s="80" t="s">
         <v>0</v>
       </c>
       <c r="P173" s="9"/>
@@ -27308,7 +27299,7 @@
         <f t="shared" si="27"/>
         <v>21</v>
       </c>
-      <c r="N581" s="77" t="s">
+      <c r="N581" s="76" t="s">
         <v>470</v>
       </c>
       <c r="O581" s="9" t="s">
@@ -27330,7 +27321,7 @@
       <c r="F582" s="32"/>
       <c r="G582" s="32"/>
       <c r="H582" s="32"/>
-      <c r="I582" s="76" t="s">
+      <c r="I582" s="75" t="s">
         <v>29</v>
       </c>
       <c r="J582" s="11">
@@ -27348,7 +27339,7 @@
         <f t="shared" si="27"/>
         <v>22</v>
       </c>
-      <c r="N582" s="77" t="s">
+      <c r="N582" s="76" t="s">
         <v>1223</v>
       </c>
       <c r="O582" s="9"/>
@@ -27361,7 +27352,7 @@
       <c r="V582" s="70" t="s">
         <v>973</v>
       </c>
-      <c r="W582" s="78"/>
+      <c r="W582" s="77"/>
     </row>
     <row r="583" spans="4:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D583" s="38"/>
@@ -31483,7 +31474,7 @@
         <f t="shared" si="33"/>
         <v>59</v>
       </c>
-      <c r="N691" s="74" t="s">
+      <c r="N691" s="73" t="s">
         <v>525</v>
       </c>
       <c r="O691" s="8"/>
@@ -34577,7 +34568,7 @@
         <f t="shared" si="37"/>
         <v>143</v>
       </c>
-      <c r="N775" s="74" t="s">
+      <c r="N775" s="73" t="s">
         <v>185</v>
       </c>
       <c r="O775" s="8"/>
@@ -36047,7 +36038,7 @@
       <c r="S814" s="9"/>
       <c r="T814" s="9"/>
       <c r="U814" s="9"/>
-      <c r="V814" s="82" t="s">
+      <c r="V814" s="81" t="s">
         <v>1049</v>
       </c>
     </row>
@@ -44204,7 +44195,7 @@
       <c r="S1033" s="9"/>
       <c r="T1033" s="9"/>
       <c r="U1033" s="9"/>
-      <c r="V1033" s="82" t="s">
+      <c r="V1033" s="81" t="s">
         <v>1224</v>
       </c>
     </row>
@@ -45769,7 +45760,7 @@
         <f t="shared" ref="M1076:M1107" si="52">+M1075+1</f>
         <v>2</v>
       </c>
-      <c r="N1076" s="74" t="s">
+      <c r="N1076" s="73" t="s">
         <v>185</v>
       </c>
       <c r="O1076" s="8"/>
@@ -50263,7 +50254,7 @@
         <f t="shared" si="58"/>
         <v>50</v>
       </c>
-      <c r="N1195" s="74" t="s">
+      <c r="N1195" s="73" t="s">
         <v>448</v>
       </c>
       <c r="O1195" s="8"/>
@@ -50749,7 +50740,7 @@
       <c r="S1208" s="9"/>
       <c r="T1208" s="9"/>
       <c r="U1208" s="9"/>
-      <c r="V1208" s="82" t="s">
+      <c r="V1208" s="81" t="s">
         <v>1225</v>
       </c>
     </row>
@@ -56874,7 +56865,7 @@
         <f t="shared" si="64"/>
         <v>61</v>
       </c>
-      <c r="N1369" s="83" t="s">
+      <c r="N1369" s="82" t="s">
         <v>218</v>
       </c>
       <c r="O1369" s="8"/>
@@ -56917,7 +56908,7 @@
         <f t="shared" si="64"/>
         <v>62</v>
       </c>
-      <c r="N1370" s="83" t="s">
+      <c r="N1370" s="82" t="s">
         <v>327</v>
       </c>
       <c r="O1370" s="8"/>
@@ -64173,7 +64164,7 @@
       <c r="U1580" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 1.6 Revised inputs from Raja - 24/01/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E081D5D2-9DCF-40C7-A385-AB2364AF588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85023E8D-45CA-49F2-BA37-073387D7ECD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
NMV 24 02 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B66D074-51EC-43D5-B173-A80735424ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.1'!$A$1:$V$1531</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5701" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5702" uniqueCount="1226">
   <si>
     <t>PS</t>
   </si>
@@ -3718,7 +3717,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3951,7 +3950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4178,6 +4177,9 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4458,13 +4460,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1472" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="U1483" sqref="U1483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -61490,7 +61492,9 @@
       <c r="R1483" s="9"/>
       <c r="S1483" s="9"/>
       <c r="T1483" s="9"/>
-      <c r="U1483" s="9"/>
+      <c r="U1483" s="83" t="s">
+        <v>56</v>
+      </c>
       <c r="V1483" s="70" t="s">
         <v>973</v>
       </c>

</xml_diff>

<commit_message>
TS 1.7 & 1.8 Ghanam Tamil - 01/03/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3C9460-E69B-44EC-BA7A-CC43807A4EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.1'!$A$1:$V$1531</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3717,7 +3719,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4460,13 +4462,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1472" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U1483" sqref="U1483"/>
+      <selection pane="bottomLeft" activeCell="N855" sqref="N855"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edits to Padam Input Templates - 29/03/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3C9460-E69B-44EC-BA7A-CC43807A4EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635B6D69-8FBE-4484-B40C-AD089077B86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4466,9 +4466,9 @@
   <dimension ref="A1:W1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1323" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N855" sqref="N855"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -64170,6 +64170,7 @@
       <c r="U1580" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V1531" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
nmv 27 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7558CF-A52E-4D44-B2EA-8F90BD3D89F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43154B6-29B0-42F3-8042-3AE8E5FCF8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5704" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5708" uniqueCount="1226">
   <si>
     <t>PS</t>
   </si>
@@ -3543,9 +3543,6 @@
   </si>
   <si>
     <t>vijA#mAtuqritiq vi - jAqmAqtuqH</t>
-  </si>
-  <si>
-    <t>syAqlAditi# syAlat</t>
   </si>
   <si>
     <t>prayaqtItiq pra - yaqtIq</t>
@@ -3794,6 +3791,9 @@
       </rPr>
       <t>ta - taqnoq</t>
     </r>
+  </si>
+  <si>
+    <t>syAqlAditi# syAqlAt</t>
   </si>
 </sst>
 </file>
@@ -4038,7 +4038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4245,6 +4245,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4529,9 +4532,9 @@
   <dimension ref="A1:W1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1266" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1323" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1271" sqref="V1271"/>
+      <selection pane="bottomLeft" activeCell="V1334" sqref="V1334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5053,7 +5056,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="T1" s="15" t="s">
         <v>78</v>
@@ -5621,7 +5624,7 @@
         <v>14</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>0</v>
@@ -6279,7 +6282,7 @@
         <v>30</v>
       </c>
       <c r="N31" s="72" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="O31" s="9" t="s">
         <v>0</v>
@@ -8604,7 +8607,7 @@
         <v>47</v>
       </c>
       <c r="N91" s="67" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="O91" s="9" t="s">
         <v>0</v>
@@ -13697,7 +13700,7 @@
         <v>48</v>
       </c>
       <c r="N238" s="73" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O238" s="8"/>
       <c r="P238" s="9"/>
@@ -25496,7 +25499,7 @@
         <v>22</v>
       </c>
       <c r="N582" s="25" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O582" s="9"/>
       <c r="P582" s="9"/>
@@ -39372,7 +39375,7 @@
         <v>39</v>
       </c>
       <c r="N998" s="62" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="O998" s="8"/>
       <c r="P998" s="9"/>
@@ -40622,7 +40625,7 @@
       <c r="T1033" s="9"/>
       <c r="U1033" s="9"/>
       <c r="V1033" s="69" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1034" spans="8:22" x14ac:dyDescent="0.25">
@@ -46514,7 +46517,7 @@
       <c r="T1208" s="9"/>
       <c r="U1208" s="9"/>
       <c r="V1208" s="69" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1209" spans="9:22" x14ac:dyDescent="0.25">
@@ -48598,7 +48601,7 @@
         <v>56</v>
       </c>
       <c r="V1271" s="69" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1272" spans="5:22" x14ac:dyDescent="0.25">
@@ -50765,8 +50768,8 @@
       <c r="R1334" s="9"/>
       <c r="S1334" s="9"/>
       <c r="T1334" s="9"/>
-      <c r="V1334" s="59" t="s">
-        <v>1169</v>
+      <c r="V1334" s="75" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="1335" spans="3:22" x14ac:dyDescent="0.25">
@@ -50874,7 +50877,7 @@
       <c r="T1337" s="9"/>
       <c r="U1337" s="9"/>
       <c r="V1337" s="59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1338" spans="3:22" x14ac:dyDescent="0.25">
@@ -50911,7 +50914,7 @@
       <c r="T1338" s="9"/>
       <c r="U1338" s="9"/>
       <c r="V1338" s="59" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1339" spans="3:22" x14ac:dyDescent="0.25">
@@ -50948,7 +50951,7 @@
       <c r="T1339" s="9"/>
       <c r="U1339" s="9"/>
       <c r="V1339" s="59" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1340" spans="3:22" x14ac:dyDescent="0.25">
@@ -51055,7 +51058,7 @@
       <c r="T1342" s="9"/>
       <c r="U1342" s="9"/>
       <c r="V1342" s="59" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1343" spans="3:22" x14ac:dyDescent="0.25">
@@ -51092,7 +51095,7 @@
       <c r="T1343" s="9"/>
       <c r="U1343" s="9"/>
       <c r="V1343" s="59" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1344" spans="3:22" x14ac:dyDescent="0.25">
@@ -51199,7 +51202,7 @@
       <c r="T1346" s="9"/>
       <c r="U1346" s="9"/>
       <c r="V1346" s="59" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1347" spans="3:22" x14ac:dyDescent="0.25">
@@ -51236,7 +51239,7 @@
       <c r="T1347" s="9"/>
       <c r="U1347" s="9"/>
       <c r="V1347" s="59" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1348" spans="3:22" x14ac:dyDescent="0.25">
@@ -51343,7 +51346,7 @@
       <c r="T1350" s="9"/>
       <c r="U1350" s="9"/>
       <c r="V1350" s="59" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1351" spans="3:22" x14ac:dyDescent="0.25">
@@ -51485,7 +51488,7 @@
       <c r="T1354" s="9"/>
       <c r="U1354" s="9"/>
       <c r="V1354" s="59" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1355" spans="3:22" x14ac:dyDescent="0.25">
@@ -51557,7 +51560,7 @@
       <c r="T1356" s="9"/>
       <c r="U1356" s="9"/>
       <c r="V1356" s="59" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1357" spans="3:22" x14ac:dyDescent="0.25">
@@ -51594,7 +51597,7 @@
       <c r="T1357" s="9"/>
       <c r="U1357" s="9"/>
       <c r="V1357" s="59" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1358" spans="3:22" x14ac:dyDescent="0.25">
@@ -51631,7 +51634,7 @@
       <c r="T1358" s="9"/>
       <c r="U1358" s="9"/>
       <c r="V1358" s="59" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1359" spans="3:22" x14ac:dyDescent="0.25">
@@ -51785,7 +51788,7 @@
       <c r="T1362" s="9"/>
       <c r="U1362" s="9"/>
       <c r="V1362" s="59" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1363" spans="3:22" x14ac:dyDescent="0.25">
@@ -52000,7 +52003,7 @@
       <c r="T1368" s="9"/>
       <c r="U1368" s="9"/>
       <c r="V1368" s="59" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1369" spans="3:22" x14ac:dyDescent="0.25">
@@ -52315,7 +52318,7 @@
       <c r="T1376" s="9"/>
       <c r="U1376" s="9"/>
       <c r="V1376" s="59" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1377" spans="3:22" x14ac:dyDescent="0.25">
@@ -52422,7 +52425,7 @@
       <c r="T1379" s="9"/>
       <c r="U1379" s="9"/>
       <c r="V1379" s="59" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1380" spans="3:22" x14ac:dyDescent="0.25">
@@ -52462,7 +52465,7 @@
       <c r="T1380" s="9"/>
       <c r="U1380" s="9"/>
       <c r="V1380" s="59" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1381" spans="3:22" x14ac:dyDescent="0.25">
@@ -52502,7 +52505,7 @@
       <c r="T1381" s="9"/>
       <c r="U1381" s="9"/>
       <c r="V1381" s="59" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1382" spans="3:22" x14ac:dyDescent="0.25">
@@ -52727,7 +52730,7 @@
       <c r="T1387" s="9"/>
       <c r="U1387" s="9"/>
       <c r="V1387" s="59" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1388" spans="3:22" x14ac:dyDescent="0.25">
@@ -52904,7 +52907,7 @@
       <c r="T1392" s="9"/>
       <c r="U1392" s="9"/>
       <c r="V1392" s="59" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1393" spans="3:22" x14ac:dyDescent="0.25">
@@ -52941,7 +52944,7 @@
       <c r="T1393" s="9"/>
       <c r="U1393" s="9"/>
       <c r="V1393" s="59" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1394" spans="3:22" x14ac:dyDescent="0.25">
@@ -53050,7 +53053,7 @@
       <c r="T1396" s="9"/>
       <c r="U1396" s="9"/>
       <c r="V1396" s="59" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1397" spans="3:22" x14ac:dyDescent="0.25">
@@ -53262,7 +53265,7 @@
       <c r="T1402" s="9"/>
       <c r="U1402" s="9"/>
       <c r="V1402" s="59" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1403" spans="3:22" x14ac:dyDescent="0.25">
@@ -53564,7 +53567,7 @@
       <c r="T1410" s="9"/>
       <c r="U1410" s="9"/>
       <c r="V1410" s="59" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1411" spans="3:22" x14ac:dyDescent="0.25">
@@ -53671,7 +53674,7 @@
       <c r="T1413" s="9"/>
       <c r="U1413" s="9"/>
       <c r="V1413" s="59" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1414" spans="3:22" x14ac:dyDescent="0.25">
@@ -53885,7 +53888,7 @@
       <c r="T1419" s="9"/>
       <c r="U1419" s="9"/>
       <c r="V1419" s="59" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1420" spans="3:22" x14ac:dyDescent="0.25">
@@ -53922,7 +53925,7 @@
       <c r="T1420" s="9"/>
       <c r="U1420" s="9"/>
       <c r="V1420" s="59" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1421" spans="3:22" x14ac:dyDescent="0.25">
@@ -54029,7 +54032,7 @@
       <c r="T1423" s="9"/>
       <c r="U1423" s="9"/>
       <c r="V1423" s="59" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1424" spans="3:22" x14ac:dyDescent="0.25">
@@ -54171,7 +54174,7 @@
       <c r="T1427" s="9"/>
       <c r="U1427" s="9"/>
       <c r="V1427" s="59" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1428" spans="2:22" x14ac:dyDescent="0.25">
@@ -54278,7 +54281,7 @@
       <c r="T1430" s="9"/>
       <c r="U1430" s="9"/>
       <c r="V1430" s="59" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1431" spans="2:22" x14ac:dyDescent="0.25">
@@ -54498,7 +54501,7 @@
       <c r="T1436" s="9"/>
       <c r="U1436" s="9"/>
       <c r="V1436" s="59" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1437" spans="2:22" x14ac:dyDescent="0.25">
@@ -54745,7 +54748,7 @@
       <c r="T1443" s="9"/>
       <c r="U1443" s="9"/>
       <c r="V1443" s="59" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1444" spans="2:22" x14ac:dyDescent="0.25">
@@ -54782,7 +54785,7 @@
       <c r="T1444" s="9"/>
       <c r="U1444" s="9"/>
       <c r="V1444" s="59" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1445" spans="2:22" x14ac:dyDescent="0.25">
@@ -55142,7 +55145,7 @@
       <c r="T1454" s="9"/>
       <c r="U1454" s="9"/>
       <c r="V1454" s="59" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1455" spans="2:22" x14ac:dyDescent="0.25">
@@ -55640,7 +55643,7 @@
       <c r="T1467" s="9"/>
       <c r="U1467" s="9"/>
       <c r="V1467" s="59" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1468" spans="3:22" x14ac:dyDescent="0.25">
@@ -55893,7 +55896,7 @@
       <c r="T1474" s="9"/>
       <c r="U1474" s="9"/>
       <c r="V1474" s="59" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1475" spans="3:22" x14ac:dyDescent="0.25">
@@ -56195,7 +56198,7 @@
       <c r="T1482" s="9"/>
       <c r="U1482" s="9"/>
       <c r="V1482" s="59" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1483" spans="3:22" x14ac:dyDescent="0.25">
@@ -56418,7 +56421,7 @@
       <c r="T1488" s="9"/>
       <c r="U1488" s="9"/>
       <c r="V1488" s="59" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1489" spans="2:22" x14ac:dyDescent="0.25">
@@ -56492,7 +56495,7 @@
       <c r="T1490" s="9"/>
       <c r="U1490" s="9"/>
       <c r="V1490" s="59" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1491" spans="2:22" x14ac:dyDescent="0.25">
@@ -56529,7 +56532,7 @@
       <c r="T1491" s="9"/>
       <c r="U1491" s="9"/>
       <c r="V1491" s="59" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1492" spans="2:22" x14ac:dyDescent="0.25">
@@ -56920,7 +56923,7 @@
       <c r="T1502" s="9"/>
       <c r="U1502" s="9"/>
       <c r="V1502" s="59" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1503" spans="2:22" x14ac:dyDescent="0.25">
@@ -57035,7 +57038,7 @@
       <c r="T1505" s="9"/>
       <c r="U1505" s="9"/>
       <c r="V1505" s="59" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1506" spans="3:22" x14ac:dyDescent="0.25">
@@ -57216,7 +57219,7 @@
       <c r="T1510" s="9"/>
       <c r="U1510" s="9"/>
       <c r="V1510" s="59" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1511" spans="3:22" x14ac:dyDescent="0.25">
@@ -57323,7 +57326,7 @@
       <c r="T1513" s="9"/>
       <c r="U1513" s="9"/>
       <c r="V1513" s="59" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1514" spans="3:22" x14ac:dyDescent="0.25">
@@ -57475,7 +57478,7 @@
       <c r="T1517" s="9"/>
       <c r="U1517" s="9"/>
       <c r="V1517" s="59" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1518" spans="3:22" x14ac:dyDescent="0.25">
@@ -57621,7 +57624,7 @@
         <v>56</v>
       </c>
       <c r="V1521" s="59" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1522" spans="2:22" x14ac:dyDescent="0.25">
@@ -57957,7 +57960,7 @@
       <c r="T1530" s="9"/>
       <c r="U1530" s="9"/>
       <c r="V1530" s="59" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="1531" spans="2:22" x14ac:dyDescent="0.25">
@@ -57994,7 +57997,7 @@
       <c r="T1531" s="9"/>
       <c r="U1531" s="9"/>
       <c r="V1531" s="59" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="1532" spans="2:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 17 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DBA159-E735-4685-AAA7-24E7EBDCB3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA21DA0-DB1B-4EB0-A051-40AA1DD0C7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3262,9 +3262,6 @@
   </si>
   <si>
     <t>svaqdhABiqriti# sva - dhABi#H</t>
-  </si>
-  <si>
-    <t>aqnuqdRuSyetya#nu anu - dRuSya#</t>
   </si>
   <si>
     <t>yaqjaqntaq iti# yajante</t>
@@ -3786,6 +3783,9 @@
   </si>
   <si>
     <t xml:space="preserve">iqndrAqgnIq  </t>
+  </si>
+  <si>
+    <t>aqnuqdRuSyetya#nu - dRuSya#</t>
   </si>
 </sst>
 </file>
@@ -4030,7 +4030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4243,6 +4243,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4526,10 +4529,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1308" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A780" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1311" sqref="V1311"/>
+      <selection pane="bottomLeft" activeCell="V784" sqref="V784"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5051,7 +5054,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="T1" s="15" t="s">
         <v>78</v>
@@ -5619,7 +5622,7 @@
         <v>14</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>0</v>
@@ -6277,7 +6280,7 @@
         <v>30</v>
       </c>
       <c r="N31" s="72" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="O31" s="9" t="s">
         <v>0</v>
@@ -8602,7 +8605,7 @@
         <v>47</v>
       </c>
       <c r="N91" s="67" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="O91" s="9" t="s">
         <v>0</v>
@@ -13695,7 +13698,7 @@
         <v>48</v>
       </c>
       <c r="N238" s="73" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="O238" s="8"/>
       <c r="P238" s="9"/>
@@ -25494,7 +25497,7 @@
         <v>22</v>
       </c>
       <c r="N582" s="25" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O582" s="9"/>
       <c r="P582" s="9"/>
@@ -32544,8 +32547,8 @@
       <c r="U792" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="V792" s="59" t="s">
-        <v>1078</v>
+      <c r="V792" s="77" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="793" spans="4:22" x14ac:dyDescent="0.25">
@@ -32579,7 +32582,7 @@
       <c r="T793" s="9"/>
       <c r="U793" s="9"/>
       <c r="V793" s="59" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="794" spans="4:22" x14ac:dyDescent="0.25">
@@ -32960,7 +32963,7 @@
       <c r="T804" s="9"/>
       <c r="U804" s="9"/>
       <c r="V804" s="59" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="805" spans="4:22" x14ac:dyDescent="0.25">
@@ -33160,7 +33163,7 @@
       <c r="T810" s="9"/>
       <c r="U810" s="9"/>
       <c r="V810" s="59" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="811" spans="4:22" x14ac:dyDescent="0.25">
@@ -33622,7 +33625,7 @@
       <c r="T824" s="9"/>
       <c r="U824" s="9"/>
       <c r="V824" s="59" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="825" spans="9:22" x14ac:dyDescent="0.25">
@@ -33722,7 +33725,7 @@
       <c r="T827" s="9"/>
       <c r="U827" s="9"/>
       <c r="V827" s="59" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="828" spans="9:22" x14ac:dyDescent="0.25">
@@ -33854,7 +33857,7 @@
       <c r="T831" s="9"/>
       <c r="U831" s="9"/>
       <c r="V831" s="59" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="832" spans="9:22" x14ac:dyDescent="0.25">
@@ -33920,7 +33923,7 @@
       <c r="T833" s="9"/>
       <c r="U833" s="9"/>
       <c r="V833" s="59" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="834" spans="4:22" x14ac:dyDescent="0.25">
@@ -34052,7 +34055,7 @@
       <c r="T837" s="9"/>
       <c r="U837" s="9"/>
       <c r="V837" s="59" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="838" spans="4:22" x14ac:dyDescent="0.25">
@@ -34086,7 +34089,7 @@
       <c r="T838" s="9"/>
       <c r="U838" s="9"/>
       <c r="V838" s="59" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="839" spans="4:22" x14ac:dyDescent="0.25">
@@ -34120,7 +34123,7 @@
       <c r="T839" s="9"/>
       <c r="U839" s="9"/>
       <c r="V839" s="59" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="840" spans="4:22" x14ac:dyDescent="0.25">
@@ -34218,7 +34221,7 @@
       <c r="T842" s="9"/>
       <c r="U842" s="9"/>
       <c r="V842" s="59" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="843" spans="4:22" x14ac:dyDescent="0.25">
@@ -34286,7 +34289,7 @@
       <c r="T844" s="9"/>
       <c r="U844" s="9"/>
       <c r="V844" s="59" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="845" spans="4:22" x14ac:dyDescent="0.25">
@@ -34355,7 +34358,7 @@
       <c r="T846" s="9"/>
       <c r="U846" s="9"/>
       <c r="V846" s="59" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="847" spans="4:22" x14ac:dyDescent="0.25">
@@ -34434,7 +34437,7 @@
         <v>55</v>
       </c>
       <c r="V848" s="59" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="849" spans="8:22" x14ac:dyDescent="0.25">
@@ -34733,7 +34736,7 @@
       <c r="T857" s="9"/>
       <c r="U857" s="9"/>
       <c r="V857" s="59" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="858" spans="8:22" x14ac:dyDescent="0.25">
@@ -34863,7 +34866,7 @@
       <c r="T861" s="9"/>
       <c r="U861" s="9"/>
       <c r="V861" s="59" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="862" spans="8:22" x14ac:dyDescent="0.25">
@@ -35057,7 +35060,7 @@
       <c r="T867" s="9"/>
       <c r="U867" s="9"/>
       <c r="V867" s="59" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="868" spans="4:22" x14ac:dyDescent="0.25">
@@ -35189,7 +35192,7 @@
       <c r="T871" s="9"/>
       <c r="U871" s="9"/>
       <c r="V871" s="59" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="872" spans="4:22" x14ac:dyDescent="0.25">
@@ -35328,7 +35331,7 @@
       </c>
       <c r="U875" s="9"/>
       <c r="V875" s="59" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="876" spans="4:22" x14ac:dyDescent="0.25">
@@ -35622,7 +35625,7 @@
       <c r="T884" s="9"/>
       <c r="U884" s="9"/>
       <c r="V884" s="59" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="885" spans="9:22" x14ac:dyDescent="0.25">
@@ -36316,7 +36319,7 @@
       <c r="T905" s="9"/>
       <c r="U905" s="9"/>
       <c r="V905" s="59" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="906" spans="4:22" x14ac:dyDescent="0.25">
@@ -36870,7 +36873,7 @@
       <c r="T921" s="9"/>
       <c r="U921" s="9"/>
       <c r="V921" s="59" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="922" spans="8:22" x14ac:dyDescent="0.25">
@@ -36936,7 +36939,7 @@
       <c r="T923" s="9"/>
       <c r="U923" s="9"/>
       <c r="V923" s="59" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="924" spans="8:22" x14ac:dyDescent="0.25">
@@ -37002,7 +37005,7 @@
       <c r="T925" s="9"/>
       <c r="U925" s="9"/>
       <c r="V925" s="59" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="926" spans="8:22" x14ac:dyDescent="0.25">
@@ -37680,7 +37683,7 @@
       <c r="T946" s="9"/>
       <c r="U946" s="9"/>
       <c r="V946" s="59" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="947" spans="9:22" x14ac:dyDescent="0.25">
@@ -37746,7 +37749,7 @@
       <c r="T948" s="9"/>
       <c r="U948" s="9"/>
       <c r="V948" s="59" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="949" spans="9:22" x14ac:dyDescent="0.25">
@@ -38004,7 +38007,7 @@
       <c r="T956" s="9"/>
       <c r="U956" s="9"/>
       <c r="V956" s="59" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="957" spans="9:22" x14ac:dyDescent="0.25">
@@ -38070,7 +38073,7 @@
       <c r="T958" s="9"/>
       <c r="U958" s="9"/>
       <c r="V958" s="59" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="959" spans="9:22" x14ac:dyDescent="0.25">
@@ -38104,7 +38107,7 @@
       <c r="T959" s="9"/>
       <c r="U959" s="9"/>
       <c r="V959" s="59" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="960" spans="9:22" x14ac:dyDescent="0.25">
@@ -38201,7 +38204,7 @@
       <c r="T962" s="9"/>
       <c r="U962" s="9"/>
       <c r="V962" s="59" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="963" spans="9:22" x14ac:dyDescent="0.25">
@@ -38555,7 +38558,7 @@
       <c r="T973" s="9"/>
       <c r="U973" s="9"/>
       <c r="V973" s="59" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="974" spans="9:22" x14ac:dyDescent="0.25">
@@ -38879,7 +38882,7 @@
       <c r="T983" s="9"/>
       <c r="U983" s="9"/>
       <c r="V983" s="59" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="984" spans="8:22" x14ac:dyDescent="0.25">
@@ -38986,7 +38989,7 @@
       <c r="T986" s="9"/>
       <c r="U986" s="9"/>
       <c r="V986" s="59" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="987" spans="8:22" x14ac:dyDescent="0.25">
@@ -39218,7 +39221,7 @@
       <c r="T993" s="9"/>
       <c r="U993" s="9"/>
       <c r="V993" s="59" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="994" spans="4:22" x14ac:dyDescent="0.25">
@@ -39316,7 +39319,7 @@
       <c r="T996" s="9"/>
       <c r="U996" s="9"/>
       <c r="V996" s="59" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="997" spans="4:22" x14ac:dyDescent="0.25">
@@ -39370,7 +39373,7 @@
         <v>39</v>
       </c>
       <c r="N998" s="62" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="O998" s="8"/>
       <c r="P998" s="9"/>
@@ -39446,7 +39449,7 @@
       <c r="T1000" s="9"/>
       <c r="U1000" s="9"/>
       <c r="V1000" s="59" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1001" spans="4:22" x14ac:dyDescent="0.25">
@@ -39591,7 +39594,7 @@
       <c r="T1004" s="9"/>
       <c r="U1004" s="9"/>
       <c r="V1004" s="59" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="1005" spans="4:22" x14ac:dyDescent="0.25">
@@ -39883,7 +39886,7 @@
       <c r="T1012" s="9"/>
       <c r="U1012" s="9"/>
       <c r="V1012" s="59" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="1013" spans="4:22" x14ac:dyDescent="0.25">
@@ -40000,7 +40003,7 @@
       <c r="T1015" s="9"/>
       <c r="U1015" s="9"/>
       <c r="V1015" s="59" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="1016" spans="4:22" x14ac:dyDescent="0.25">
@@ -40066,7 +40069,7 @@
       <c r="T1017" s="9"/>
       <c r="U1017" s="9"/>
       <c r="V1017" s="59" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="1018" spans="4:22" x14ac:dyDescent="0.25">
@@ -40277,7 +40280,7 @@
       <c r="T1023" s="9"/>
       <c r="U1023" s="9"/>
       <c r="V1023" s="59" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="1024" spans="4:22" x14ac:dyDescent="0.25">
@@ -40586,7 +40589,7 @@
       <c r="T1032" s="9"/>
       <c r="U1032" s="9"/>
       <c r="V1032" s="59" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1033" spans="8:22" x14ac:dyDescent="0.25">
@@ -40620,7 +40623,7 @@
       <c r="T1033" s="9"/>
       <c r="U1033" s="9"/>
       <c r="V1033" s="69" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1034" spans="8:22" x14ac:dyDescent="0.25">
@@ -40718,7 +40721,7 @@
       <c r="T1036" s="9"/>
       <c r="U1036" s="9"/>
       <c r="V1036" s="59" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="1037" spans="8:22" x14ac:dyDescent="0.25">
@@ -40960,7 +40963,7 @@
       <c r="T1043" s="9"/>
       <c r="U1043" s="9"/>
       <c r="V1043" s="59" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="1044" spans="8:22" x14ac:dyDescent="0.25">
@@ -41218,7 +41221,7 @@
       <c r="T1051" s="9"/>
       <c r="U1051" s="9"/>
       <c r="V1051" s="59" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1052" spans="8:22" x14ac:dyDescent="0.25">
@@ -41604,7 +41607,7 @@
       <c r="T1063" s="9"/>
       <c r="U1063" s="9"/>
       <c r="V1063" s="59" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="1064" spans="9:22" x14ac:dyDescent="0.25">
@@ -41702,7 +41705,7 @@
       <c r="T1066" s="9"/>
       <c r="U1066" s="9"/>
       <c r="V1066" s="59" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1067" spans="9:22" x14ac:dyDescent="0.25">
@@ -41964,7 +41967,7 @@
       <c r="T1074" s="9"/>
       <c r="U1074" s="9"/>
       <c r="V1074" s="59" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1075" spans="4:22" x14ac:dyDescent="0.25">
@@ -42230,7 +42233,7 @@
       <c r="T1082" s="9"/>
       <c r="U1082" s="9"/>
       <c r="V1082" s="59" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1083" spans="4:22" x14ac:dyDescent="0.25">
@@ -42516,7 +42519,7 @@
       <c r="T1090" s="9"/>
       <c r="U1090" s="9"/>
       <c r="V1090" s="59" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1091" spans="8:22" x14ac:dyDescent="0.25">
@@ -42792,7 +42795,7 @@
         <v>56</v>
       </c>
       <c r="V1098" s="59" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1099" spans="8:22" x14ac:dyDescent="0.25">
@@ -43244,7 +43247,7 @@
       <c r="T1111" s="9"/>
       <c r="U1111" s="9"/>
       <c r="V1111" s="59" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1112" spans="8:22" x14ac:dyDescent="0.25">
@@ -43536,7 +43539,7 @@
       <c r="T1120" s="9"/>
       <c r="U1120" s="9"/>
       <c r="V1120" s="59" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1121" spans="2:22" x14ac:dyDescent="0.25">
@@ -43645,7 +43648,7 @@
       <c r="T1123" s="9"/>
       <c r="U1123" s="9"/>
       <c r="V1123" s="59" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1124" spans="2:22" x14ac:dyDescent="0.25">
@@ -43746,7 +43749,7 @@
       <c r="T1126" s="9"/>
       <c r="U1126" s="9"/>
       <c r="V1126" s="59" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1127" spans="2:22" x14ac:dyDescent="0.25">
@@ -43780,7 +43783,7 @@
       <c r="T1127" s="9"/>
       <c r="U1127" s="9"/>
       <c r="V1127" s="59" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1128" spans="2:22" x14ac:dyDescent="0.25">
@@ -44009,7 +44012,7 @@
       <c r="T1134" s="9"/>
       <c r="U1134" s="9"/>
       <c r="V1134" s="59" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1135" spans="2:22" x14ac:dyDescent="0.25">
@@ -44118,7 +44121,7 @@
       <c r="T1137" s="9"/>
       <c r="U1137" s="9"/>
       <c r="V1137" s="59" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1138" spans="8:22" x14ac:dyDescent="0.25">
@@ -44381,7 +44384,7 @@
       <c r="T1145" s="9"/>
       <c r="U1145" s="9"/>
       <c r="V1145" s="59" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1146" spans="8:22" x14ac:dyDescent="0.25">
@@ -44478,7 +44481,7 @@
       <c r="T1148" s="9"/>
       <c r="U1148" s="9"/>
       <c r="V1148" s="59" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1149" spans="8:22" x14ac:dyDescent="0.25">
@@ -44515,7 +44518,7 @@
       <c r="T1149" s="9"/>
       <c r="U1149" s="9"/>
       <c r="V1149" s="59" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1150" spans="8:22" x14ac:dyDescent="0.25">
@@ -44589,7 +44592,7 @@
       <c r="T1151" s="9"/>
       <c r="U1151" s="9"/>
       <c r="V1151" s="59" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1152" spans="8:22" x14ac:dyDescent="0.25">
@@ -44780,7 +44783,7 @@
       <c r="T1156" s="9"/>
       <c r="U1156" s="9"/>
       <c r="V1156" s="59" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1157" spans="4:22" x14ac:dyDescent="0.25">
@@ -44865,7 +44868,7 @@
       </c>
       <c r="U1158" s="9"/>
       <c r="V1158" s="59" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1159" spans="4:22" x14ac:dyDescent="0.25">
@@ -44899,7 +44902,7 @@
       <c r="T1159" s="9"/>
       <c r="U1159" s="9"/>
       <c r="V1159" s="59" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1160" spans="4:22" x14ac:dyDescent="0.25">
@@ -44965,7 +44968,7 @@
       <c r="T1161" s="9"/>
       <c r="U1161" s="9"/>
       <c r="V1161" s="59" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1162" spans="4:22" x14ac:dyDescent="0.25">
@@ -45095,7 +45098,7 @@
       <c r="T1165" s="9"/>
       <c r="U1165" s="9"/>
       <c r="V1165" s="59" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1166" spans="4:22" x14ac:dyDescent="0.25">
@@ -45203,7 +45206,7 @@
       <c r="T1168" s="9"/>
       <c r="U1168" s="9"/>
       <c r="V1168" s="59" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1169" spans="2:22" x14ac:dyDescent="0.25">
@@ -45338,7 +45341,7 @@
       <c r="T1172" s="9"/>
       <c r="U1172" s="9"/>
       <c r="V1172" s="59" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1173" spans="2:22" x14ac:dyDescent="0.25">
@@ -45372,7 +45375,7 @@
       <c r="T1173" s="9"/>
       <c r="U1173" s="9"/>
       <c r="V1173" s="59" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1174" spans="2:22" x14ac:dyDescent="0.25">
@@ -45662,7 +45665,7 @@
       <c r="T1182" s="9"/>
       <c r="U1182" s="9"/>
       <c r="V1182" s="59" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="1183" spans="2:22" x14ac:dyDescent="0.25">
@@ -46284,7 +46287,7 @@
       <c r="T1201" s="9"/>
       <c r="U1201" s="9"/>
       <c r="V1201" s="59" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1202" spans="9:22" x14ac:dyDescent="0.25">
@@ -46318,7 +46321,7 @@
       <c r="T1202" s="9"/>
       <c r="U1202" s="9"/>
       <c r="V1202" s="59" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1203" spans="9:22" x14ac:dyDescent="0.25">
@@ -46512,7 +46515,7 @@
       <c r="T1208" s="9"/>
       <c r="U1208" s="9"/>
       <c r="V1208" s="69" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1209" spans="9:22" x14ac:dyDescent="0.25">
@@ -46802,7 +46805,7 @@
       <c r="T1217" s="9"/>
       <c r="U1217" s="9"/>
       <c r="V1217" s="59" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1218" spans="8:22" x14ac:dyDescent="0.25">
@@ -46836,7 +46839,7 @@
       <c r="T1218" s="9"/>
       <c r="U1218" s="9"/>
       <c r="V1218" s="59" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1219" spans="8:22" x14ac:dyDescent="0.25">
@@ -46934,7 +46937,7 @@
       <c r="T1221" s="9"/>
       <c r="U1221" s="9"/>
       <c r="V1221" s="59" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1222" spans="8:22" x14ac:dyDescent="0.25">
@@ -46968,7 +46971,7 @@
       <c r="T1222" s="9"/>
       <c r="U1222" s="9"/>
       <c r="V1222" s="59" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1223" spans="8:22" x14ac:dyDescent="0.25">
@@ -47339,7 +47342,7 @@
       <c r="T1233" s="9"/>
       <c r="U1233" s="9"/>
       <c r="V1233" s="59" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1234" spans="8:22" x14ac:dyDescent="0.25">
@@ -47537,7 +47540,7 @@
       <c r="T1239" s="9"/>
       <c r="U1239" s="9"/>
       <c r="V1239" s="59" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1240" spans="8:22" x14ac:dyDescent="0.25">
@@ -47667,7 +47670,7 @@
       <c r="T1243" s="9"/>
       <c r="U1243" s="9"/>
       <c r="V1243" s="59" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1244" spans="8:22" x14ac:dyDescent="0.25">
@@ -47701,7 +47704,7 @@
       <c r="T1244" s="9"/>
       <c r="U1244" s="9"/>
       <c r="V1244" s="59" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1245" spans="8:22" x14ac:dyDescent="0.25">
@@ -47961,7 +47964,7 @@
       <c r="T1252" s="9"/>
       <c r="U1252" s="9"/>
       <c r="V1252" s="59" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1253" spans="9:22" x14ac:dyDescent="0.25">
@@ -48155,7 +48158,7 @@
       <c r="T1258" s="9"/>
       <c r="U1258" s="9"/>
       <c r="V1258" s="59" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1259" spans="9:22" x14ac:dyDescent="0.25">
@@ -48285,7 +48288,7 @@
       <c r="T1262" s="9"/>
       <c r="U1262" s="9"/>
       <c r="V1262" s="59" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1263" spans="9:22" x14ac:dyDescent="0.25">
@@ -48554,7 +48557,7 @@
         <v>62</v>
       </c>
       <c r="V1270" s="59" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1271" spans="5:22" x14ac:dyDescent="0.25">
@@ -48596,7 +48599,7 @@
         <v>56</v>
       </c>
       <c r="V1271" s="69" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1272" spans="5:22" x14ac:dyDescent="0.25">
@@ -48790,7 +48793,7 @@
       <c r="T1277" s="9"/>
       <c r="U1277" s="9"/>
       <c r="V1277" s="59" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1278" spans="5:22" x14ac:dyDescent="0.25">
@@ -48856,7 +48859,7 @@
       <c r="T1279" s="9"/>
       <c r="U1279" s="9"/>
       <c r="V1279" s="59" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1280" spans="5:22" x14ac:dyDescent="0.25">
@@ -48922,7 +48925,7 @@
       <c r="T1281" s="9"/>
       <c r="U1281" s="9"/>
       <c r="V1281" s="59" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="1282" spans="9:22" x14ac:dyDescent="0.25">
@@ -48988,7 +48991,7 @@
       <c r="T1283" s="9"/>
       <c r="U1283" s="9"/>
       <c r="V1283" s="59" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1284" spans="9:22" x14ac:dyDescent="0.25">
@@ -49150,7 +49153,7 @@
       <c r="T1288" s="9"/>
       <c r="U1288" s="9"/>
       <c r="V1288" s="59" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1289" spans="9:22" x14ac:dyDescent="0.25">
@@ -49280,7 +49283,7 @@
       <c r="T1292" s="9"/>
       <c r="U1292" s="9"/>
       <c r="V1292" s="59" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1293" spans="9:22" x14ac:dyDescent="0.25">
@@ -49798,7 +49801,7 @@
       <c r="T1308" s="9"/>
       <c r="U1308" s="9"/>
       <c r="V1308" s="59" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1309" spans="3:22" x14ac:dyDescent="0.25">
@@ -49910,7 +49913,7 @@
         <v>3</v>
       </c>
       <c r="N1311" s="76" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="O1311" s="9" t="s">
         <v>49</v>
@@ -49922,7 +49925,7 @@
       <c r="T1311" s="9"/>
       <c r="U1311" s="9"/>
       <c r="V1311" s="59" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1312" spans="3:22" x14ac:dyDescent="0.25">
@@ -50099,7 +50102,7 @@
       <c r="T1316" s="9"/>
       <c r="U1316" s="9"/>
       <c r="V1316" s="59" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1317" spans="3:22" x14ac:dyDescent="0.25">
@@ -50416,7 +50419,7 @@
       <c r="T1325" s="9"/>
       <c r="U1325" s="9"/>
       <c r="V1325" s="59" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1326" spans="3:22" x14ac:dyDescent="0.25">
@@ -50532,7 +50535,7 @@
       <c r="T1328" s="9"/>
       <c r="U1328" s="9"/>
       <c r="V1328" s="59" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1329" spans="3:22" x14ac:dyDescent="0.25">
@@ -50610,7 +50613,7 @@
       <c r="T1330" s="9"/>
       <c r="U1330" s="9"/>
       <c r="V1330" s="59" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="1331" spans="3:22" x14ac:dyDescent="0.25">
@@ -50764,7 +50767,7 @@
       <c r="S1334" s="9"/>
       <c r="T1334" s="9"/>
       <c r="V1334" s="75" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1335" spans="3:22" x14ac:dyDescent="0.25">
@@ -50872,7 +50875,7 @@
       <c r="T1337" s="9"/>
       <c r="U1337" s="9"/>
       <c r="V1337" s="59" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1338" spans="3:22" x14ac:dyDescent="0.25">
@@ -50909,7 +50912,7 @@
       <c r="T1338" s="9"/>
       <c r="U1338" s="9"/>
       <c r="V1338" s="59" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1339" spans="3:22" x14ac:dyDescent="0.25">
@@ -50946,7 +50949,7 @@
       <c r="T1339" s="9"/>
       <c r="U1339" s="9"/>
       <c r="V1339" s="59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1340" spans="3:22" x14ac:dyDescent="0.25">
@@ -51053,7 +51056,7 @@
       <c r="T1342" s="9"/>
       <c r="U1342" s="9"/>
       <c r="V1342" s="59" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1343" spans="3:22" x14ac:dyDescent="0.25">
@@ -51090,7 +51093,7 @@
       <c r="T1343" s="9"/>
       <c r="U1343" s="9"/>
       <c r="V1343" s="59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1344" spans="3:22" x14ac:dyDescent="0.25">
@@ -51197,7 +51200,7 @@
       <c r="T1346" s="9"/>
       <c r="U1346" s="9"/>
       <c r="V1346" s="59" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1347" spans="3:22" x14ac:dyDescent="0.25">
@@ -51234,7 +51237,7 @@
       <c r="T1347" s="9"/>
       <c r="U1347" s="9"/>
       <c r="V1347" s="59" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1348" spans="3:22" x14ac:dyDescent="0.25">
@@ -51341,7 +51344,7 @@
       <c r="T1350" s="9"/>
       <c r="U1350" s="9"/>
       <c r="V1350" s="59" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1351" spans="3:22" x14ac:dyDescent="0.25">
@@ -51483,7 +51486,7 @@
       <c r="T1354" s="9"/>
       <c r="U1354" s="9"/>
       <c r="V1354" s="59" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1355" spans="3:22" x14ac:dyDescent="0.25">
@@ -51555,7 +51558,7 @@
       <c r="T1356" s="9"/>
       <c r="U1356" s="9"/>
       <c r="V1356" s="59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1357" spans="3:22" x14ac:dyDescent="0.25">
@@ -51592,7 +51595,7 @@
       <c r="T1357" s="9"/>
       <c r="U1357" s="9"/>
       <c r="V1357" s="59" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1358" spans="3:22" x14ac:dyDescent="0.25">
@@ -51629,7 +51632,7 @@
       <c r="T1358" s="9"/>
       <c r="U1358" s="9"/>
       <c r="V1358" s="59" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1359" spans="3:22" x14ac:dyDescent="0.25">
@@ -51783,7 +51786,7 @@
       <c r="T1362" s="9"/>
       <c r="U1362" s="9"/>
       <c r="V1362" s="59" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1363" spans="3:22" x14ac:dyDescent="0.25">
@@ -51998,7 +52001,7 @@
       <c r="T1368" s="9"/>
       <c r="U1368" s="9"/>
       <c r="V1368" s="59" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1369" spans="3:22" x14ac:dyDescent="0.25">
@@ -52313,7 +52316,7 @@
       <c r="T1376" s="9"/>
       <c r="U1376" s="9"/>
       <c r="V1376" s="59" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1377" spans="3:22" x14ac:dyDescent="0.25">
@@ -52420,7 +52423,7 @@
       <c r="T1379" s="9"/>
       <c r="U1379" s="9"/>
       <c r="V1379" s="59" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1380" spans="3:22" x14ac:dyDescent="0.25">
@@ -52460,7 +52463,7 @@
       <c r="T1380" s="9"/>
       <c r="U1380" s="9"/>
       <c r="V1380" s="59" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1381" spans="3:22" x14ac:dyDescent="0.25">
@@ -52500,7 +52503,7 @@
       <c r="T1381" s="9"/>
       <c r="U1381" s="9"/>
       <c r="V1381" s="59" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1382" spans="3:22" x14ac:dyDescent="0.25">
@@ -52725,7 +52728,7 @@
       <c r="T1387" s="9"/>
       <c r="U1387" s="9"/>
       <c r="V1387" s="59" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1388" spans="3:22" x14ac:dyDescent="0.25">
@@ -52902,7 +52905,7 @@
       <c r="T1392" s="9"/>
       <c r="U1392" s="9"/>
       <c r="V1392" s="59" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1393" spans="3:22" x14ac:dyDescent="0.25">
@@ -52939,7 +52942,7 @@
       <c r="T1393" s="9"/>
       <c r="U1393" s="9"/>
       <c r="V1393" s="59" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1394" spans="3:22" x14ac:dyDescent="0.25">
@@ -53048,7 +53051,7 @@
       <c r="T1396" s="9"/>
       <c r="U1396" s="9"/>
       <c r="V1396" s="59" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1397" spans="3:22" x14ac:dyDescent="0.25">
@@ -53260,7 +53263,7 @@
       <c r="T1402" s="9"/>
       <c r="U1402" s="9"/>
       <c r="V1402" s="59" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1403" spans="3:22" x14ac:dyDescent="0.25">
@@ -53562,7 +53565,7 @@
       <c r="T1410" s="9"/>
       <c r="U1410" s="9"/>
       <c r="V1410" s="59" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1411" spans="3:22" x14ac:dyDescent="0.25">
@@ -53669,7 +53672,7 @@
       <c r="T1413" s="9"/>
       <c r="U1413" s="9"/>
       <c r="V1413" s="59" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1414" spans="3:22" x14ac:dyDescent="0.25">
@@ -53883,7 +53886,7 @@
       <c r="T1419" s="9"/>
       <c r="U1419" s="9"/>
       <c r="V1419" s="59" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1420" spans="3:22" x14ac:dyDescent="0.25">
@@ -53920,7 +53923,7 @@
       <c r="T1420" s="9"/>
       <c r="U1420" s="9"/>
       <c r="V1420" s="59" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1421" spans="3:22" x14ac:dyDescent="0.25">
@@ -54027,7 +54030,7 @@
       <c r="T1423" s="9"/>
       <c r="U1423" s="9"/>
       <c r="V1423" s="59" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1424" spans="3:22" x14ac:dyDescent="0.25">
@@ -54169,7 +54172,7 @@
       <c r="T1427" s="9"/>
       <c r="U1427" s="9"/>
       <c r="V1427" s="59" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1428" spans="2:22" x14ac:dyDescent="0.25">
@@ -54276,7 +54279,7 @@
       <c r="T1430" s="9"/>
       <c r="U1430" s="9"/>
       <c r="V1430" s="59" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1431" spans="2:22" x14ac:dyDescent="0.25">
@@ -54496,7 +54499,7 @@
       <c r="T1436" s="9"/>
       <c r="U1436" s="9"/>
       <c r="V1436" s="59" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1437" spans="2:22" x14ac:dyDescent="0.25">
@@ -54743,7 +54746,7 @@
       <c r="T1443" s="9"/>
       <c r="U1443" s="9"/>
       <c r="V1443" s="59" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1444" spans="2:22" x14ac:dyDescent="0.25">
@@ -54780,7 +54783,7 @@
       <c r="T1444" s="9"/>
       <c r="U1444" s="9"/>
       <c r="V1444" s="59" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1445" spans="2:22" x14ac:dyDescent="0.25">
@@ -55140,7 +55143,7 @@
       <c r="T1454" s="9"/>
       <c r="U1454" s="9"/>
       <c r="V1454" s="59" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1455" spans="2:22" x14ac:dyDescent="0.25">
@@ -55638,7 +55641,7 @@
       <c r="T1467" s="9"/>
       <c r="U1467" s="9"/>
       <c r="V1467" s="59" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1468" spans="3:22" x14ac:dyDescent="0.25">
@@ -55891,7 +55894,7 @@
       <c r="T1474" s="9"/>
       <c r="U1474" s="9"/>
       <c r="V1474" s="59" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1475" spans="3:22" x14ac:dyDescent="0.25">
@@ -56193,7 +56196,7 @@
       <c r="T1482" s="9"/>
       <c r="U1482" s="9"/>
       <c r="V1482" s="59" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1483" spans="3:22" x14ac:dyDescent="0.25">
@@ -56416,7 +56419,7 @@
       <c r="T1488" s="9"/>
       <c r="U1488" s="9"/>
       <c r="V1488" s="59" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1489" spans="2:22" x14ac:dyDescent="0.25">
@@ -56490,7 +56493,7 @@
       <c r="T1490" s="9"/>
       <c r="U1490" s="9"/>
       <c r="V1490" s="59" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1491" spans="2:22" x14ac:dyDescent="0.25">
@@ -56527,7 +56530,7 @@
       <c r="T1491" s="9"/>
       <c r="U1491" s="9"/>
       <c r="V1491" s="59" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1492" spans="2:22" x14ac:dyDescent="0.25">
@@ -56918,7 +56921,7 @@
       <c r="T1502" s="9"/>
       <c r="U1502" s="9"/>
       <c r="V1502" s="59" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1503" spans="2:22" x14ac:dyDescent="0.25">
@@ -57033,7 +57036,7 @@
       <c r="T1505" s="9"/>
       <c r="U1505" s="9"/>
       <c r="V1505" s="59" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1506" spans="3:22" x14ac:dyDescent="0.25">
@@ -57214,7 +57217,7 @@
       <c r="T1510" s="9"/>
       <c r="U1510" s="9"/>
       <c r="V1510" s="59" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1511" spans="3:22" x14ac:dyDescent="0.25">
@@ -57321,7 +57324,7 @@
       <c r="T1513" s="9"/>
       <c r="U1513" s="9"/>
       <c r="V1513" s="59" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1514" spans="3:22" x14ac:dyDescent="0.25">
@@ -57473,7 +57476,7 @@
       <c r="T1517" s="9"/>
       <c r="U1517" s="9"/>
       <c r="V1517" s="59" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1518" spans="3:22" x14ac:dyDescent="0.25">
@@ -57619,7 +57622,7 @@
         <v>56</v>
       </c>
       <c r="V1521" s="59" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1522" spans="2:22" x14ac:dyDescent="0.25">
@@ -57955,7 +57958,7 @@
       <c r="T1530" s="9"/>
       <c r="U1530" s="9"/>
       <c r="V1530" s="59" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1531" spans="2:22" x14ac:dyDescent="0.25">
@@ -57992,7 +57995,7 @@
       <c r="T1531" s="9"/>
       <c r="U1531" s="9"/>
       <c r="V1531" s="59" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1532" spans="2:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 07 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA21DA0-DB1B-4EB0-A051-40AA1DD0C7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DB9960-E4EA-4ED0-8B9C-DD330D4134A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4529,10 +4529,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A780" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V784" sqref="V784"/>
+      <selection pane="bottomLeft" activeCell="N1333" sqref="N1333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
nmv 10 03 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DB9960-E4EA-4ED0-8B9C-DD330D4134A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A09A868-6FEA-4C4E-91F1-7FCB32119284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5704" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="1226">
   <si>
     <t>PS</t>
   </si>
@@ -3133,9 +3133,6 @@
   </si>
   <si>
     <t>prAqNAyeti# pra - aqnAya#</t>
-  </si>
-  <si>
-    <t>aqpAqnAtye#pa - aqnAya#</t>
   </si>
   <si>
     <t>vyAqnAyeti# vi - aqnAya#</t>
@@ -3786,6 +3783,9 @@
   </si>
   <si>
     <t>aqnuqdRuSyetya#nu - dRuSya#</t>
+  </si>
+  <si>
+    <t>aqpAqnAyetya#pa - aqnAya#</t>
   </si>
 </sst>
 </file>
@@ -4529,10 +4529,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1333" sqref="N1333"/>
+      <selection pane="bottomLeft" activeCell="T450" sqref="T450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5054,7 +5054,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="T1" s="15" t="s">
         <v>78</v>
@@ -5622,7 +5622,7 @@
         <v>14</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>0</v>
@@ -6280,7 +6280,7 @@
         <v>30</v>
       </c>
       <c r="N31" s="72" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O31" s="9" t="s">
         <v>0</v>
@@ -8605,7 +8605,7 @@
         <v>47</v>
       </c>
       <c r="N91" s="67" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="O91" s="9" t="s">
         <v>0</v>
@@ -13698,7 +13698,7 @@
         <v>48</v>
       </c>
       <c r="N238" s="73" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="O238" s="8"/>
       <c r="P238" s="9"/>
@@ -20928,8 +20928,8 @@
       <c r="S448" s="9"/>
       <c r="T448" s="9"/>
       <c r="U448" s="9"/>
-      <c r="V448" s="59" t="s">
-        <v>1035</v>
+      <c r="V448" s="77" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="449" spans="2:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -20997,7 +20997,7 @@
       <c r="T450" s="9"/>
       <c r="U450" s="9"/>
       <c r="V450" s="59" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="451" spans="2:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -21133,7 +21133,7 @@
       <c r="T454" s="9"/>
       <c r="U454" s="9"/>
       <c r="V454" s="59" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="455" spans="2:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -21687,7 +21687,7 @@
       <c r="T470" s="9"/>
       <c r="U470" s="9"/>
       <c r="V470" s="59" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="471" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -21800,7 +21800,7 @@
       <c r="T473" s="9"/>
       <c r="U473" s="9"/>
       <c r="V473" s="59" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="474" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -21903,7 +21903,7 @@
       <c r="T476" s="9"/>
       <c r="U476" s="9"/>
       <c r="V476" s="59" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="477" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -21971,7 +21971,7 @@
       <c r="T478" s="9"/>
       <c r="U478" s="9"/>
       <c r="V478" s="59" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="479" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -22039,7 +22039,7 @@
       <c r="T480" s="9"/>
       <c r="U480" s="9"/>
       <c r="V480" s="59" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="481" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -22305,7 +22305,7 @@
       <c r="T488" s="9"/>
       <c r="U488" s="9"/>
       <c r="V488" s="59" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="489" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -22373,7 +22373,7 @@
       <c r="T490" s="9"/>
       <c r="U490" s="9"/>
       <c r="V490" s="59" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="491" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -22674,7 +22674,7 @@
       <c r="T499" s="9"/>
       <c r="U499" s="9"/>
       <c r="V499" s="59" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="500" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -22742,7 +22742,7 @@
       <c r="T501" s="9"/>
       <c r="U501" s="9"/>
       <c r="V501" s="59" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="502" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -22810,7 +22810,7 @@
       <c r="T503" s="9"/>
       <c r="U503" s="9"/>
       <c r="V503" s="59" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="504" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -23243,7 +23243,7 @@
       <c r="T516" s="9"/>
       <c r="U516" s="9"/>
       <c r="V516" s="59" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="517" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -23610,7 +23610,7 @@
       <c r="T527" s="9"/>
       <c r="U527" s="9"/>
       <c r="V527" s="59" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="528" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -23678,7 +23678,7 @@
       <c r="T529" s="9"/>
       <c r="U529" s="9"/>
       <c r="V529" s="59" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="530" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -23913,7 +23913,7 @@
       <c r="T536" s="9"/>
       <c r="U536" s="9"/>
       <c r="V536" s="59" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="537" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -24047,7 +24047,7 @@
       <c r="T540" s="9"/>
       <c r="U540" s="9"/>
       <c r="V540" s="59" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="541" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -24447,7 +24447,7 @@
       <c r="T552" s="9"/>
       <c r="U552" s="9"/>
       <c r="V552" s="59" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="553" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -24482,7 +24482,7 @@
       <c r="T553" s="9"/>
       <c r="U553" s="9"/>
       <c r="V553" s="59" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="554" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -24657,7 +24657,7 @@
       <c r="T558" s="9"/>
       <c r="U558" s="9"/>
       <c r="V558" s="59" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="559" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -24733,7 +24733,7 @@
       <c r="T560" s="9"/>
       <c r="U560" s="9"/>
       <c r="V560" s="59" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="561" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -24911,7 +24911,7 @@
         <v>55</v>
       </c>
       <c r="V565" s="59" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="566" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -25189,7 +25189,7 @@
       <c r="T573" s="9"/>
       <c r="U573" s="9"/>
       <c r="V573" s="59" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="574" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -25225,7 +25225,7 @@
       <c r="T574" s="9"/>
       <c r="U574" s="9"/>
       <c r="V574" s="59" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="575" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -25295,7 +25295,7 @@
       <c r="T576" s="9"/>
       <c r="U576" s="9"/>
       <c r="V576" s="59" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="577" spans="4:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -25367,7 +25367,7 @@
       <c r="T578" s="9"/>
       <c r="U578" s="9"/>
       <c r="V578" s="59" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="579" spans="4:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -25473,7 +25473,7 @@
       <c r="T581" s="9"/>
       <c r="U581" s="9"/>
       <c r="V581" s="59" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="582" spans="4:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -25497,7 +25497,7 @@
         <v>22</v>
       </c>
       <c r="N582" s="25" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="O582" s="9"/>
       <c r="P582" s="9"/>
@@ -25956,7 +25956,7 @@
       <c r="T595" s="9"/>
       <c r="U595" s="9"/>
       <c r="V595" s="59" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="596" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -26128,7 +26128,7 @@
       <c r="T600" s="9"/>
       <c r="U600" s="9"/>
       <c r="V600" s="59" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="601" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -26266,7 +26266,7 @@
       <c r="T604" s="9"/>
       <c r="U604" s="9"/>
       <c r="V604" s="59" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="605" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -26336,7 +26336,7 @@
       <c r="T606" s="9"/>
       <c r="U606" s="9"/>
       <c r="V606" s="59" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="607" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27246,7 +27246,7 @@
       <c r="T632" s="22"/>
       <c r="U632" s="22"/>
       <c r="V632" s="59" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="633" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27480,7 +27480,7 @@
       <c r="T639" s="9"/>
       <c r="U639" s="9"/>
       <c r="V639" s="59" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="640" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27515,7 +27515,7 @@
       <c r="T640" s="9"/>
       <c r="U640" s="9"/>
       <c r="V640" s="59" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="641" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27616,7 +27616,7 @@
       <c r="T643" s="9"/>
       <c r="U643" s="9"/>
       <c r="V643" s="59" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="644" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27684,7 +27684,7 @@
       <c r="T645" s="9"/>
       <c r="U645" s="9"/>
       <c r="V645" s="59" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="646" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27896,7 +27896,7 @@
       <c r="T651" s="9"/>
       <c r="U651" s="9"/>
       <c r="V651" s="59" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="652" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -28069,7 +28069,7 @@
       <c r="T656" s="9"/>
       <c r="U656" s="9"/>
       <c r="V656" s="59" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="657" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -28339,7 +28339,7 @@
       <c r="T664" s="9"/>
       <c r="U664" s="9"/>
       <c r="V664" s="59" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="665" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -28792,7 +28792,7 @@
       <c r="T678" s="9"/>
       <c r="U678" s="9"/>
       <c r="V678" s="59" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="679" spans="9:22" x14ac:dyDescent="0.25">
@@ -28890,7 +28890,7 @@
       <c r="T681" s="9"/>
       <c r="U681" s="9"/>
       <c r="V681" s="59" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="682" spans="9:22" x14ac:dyDescent="0.25">
@@ -28988,7 +28988,7 @@
       <c r="T684" s="9"/>
       <c r="U684" s="9"/>
       <c r="V684" s="59" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="685" spans="9:22" x14ac:dyDescent="0.25">
@@ -29250,7 +29250,7 @@
       <c r="T692" s="9"/>
       <c r="U692" s="9"/>
       <c r="V692" s="59" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="693" spans="2:22" x14ac:dyDescent="0.25">
@@ -29703,7 +29703,7 @@
       <c r="T706" s="9"/>
       <c r="U706" s="9"/>
       <c r="V706" s="59" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="707" spans="4:22" x14ac:dyDescent="0.25">
@@ -29801,7 +29801,7 @@
       <c r="T709" s="9"/>
       <c r="U709" s="9"/>
       <c r="V709" s="59" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="710" spans="4:22" x14ac:dyDescent="0.25">
@@ -29899,7 +29899,7 @@
       <c r="T712" s="9"/>
       <c r="U712" s="9"/>
       <c r="V712" s="59" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="713" spans="4:22" x14ac:dyDescent="0.25">
@@ -30164,7 +30164,7 @@
       <c r="T720" s="9"/>
       <c r="U720" s="9"/>
       <c r="V720" s="59" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="721" spans="2:22" x14ac:dyDescent="0.25">
@@ -31654,7 +31654,7 @@
       <c r="T765" s="9"/>
       <c r="U765" s="9"/>
       <c r="V765" s="59" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="766" spans="8:22" x14ac:dyDescent="0.25">
@@ -31720,7 +31720,7 @@
       <c r="T767" s="9"/>
       <c r="U767" s="9"/>
       <c r="V767" s="59" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="768" spans="8:22" x14ac:dyDescent="0.25">
@@ -31852,7 +31852,7 @@
       <c r="T771" s="9"/>
       <c r="U771" s="9"/>
       <c r="V771" s="59" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="772" spans="6:22" x14ac:dyDescent="0.25">
@@ -32182,7 +32182,7 @@
       <c r="T781" s="9"/>
       <c r="U781" s="9"/>
       <c r="V781" s="59" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="782" spans="6:22" x14ac:dyDescent="0.25">
@@ -32216,7 +32216,7 @@
       <c r="T782" s="9"/>
       <c r="U782" s="9"/>
       <c r="V782" s="59" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="783" spans="6:22" x14ac:dyDescent="0.25">
@@ -32250,7 +32250,7 @@
       <c r="T783" s="9"/>
       <c r="U783" s="9"/>
       <c r="V783" s="59" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="784" spans="6:22" x14ac:dyDescent="0.25">
@@ -32316,7 +32316,7 @@
       <c r="T785" s="9"/>
       <c r="U785" s="9"/>
       <c r="V785" s="59" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="786" spans="4:22" x14ac:dyDescent="0.25">
@@ -32446,7 +32446,7 @@
       <c r="T789" s="9"/>
       <c r="U789" s="9"/>
       <c r="V789" s="59" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="790" spans="4:22" x14ac:dyDescent="0.25">
@@ -32548,7 +32548,7 @@
         <v>55</v>
       </c>
       <c r="V792" s="77" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="793" spans="4:22" x14ac:dyDescent="0.25">
@@ -32582,7 +32582,7 @@
       <c r="T793" s="9"/>
       <c r="U793" s="9"/>
       <c r="V793" s="59" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="794" spans="4:22" x14ac:dyDescent="0.25">
@@ -32963,7 +32963,7 @@
       <c r="T804" s="9"/>
       <c r="U804" s="9"/>
       <c r="V804" s="59" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="805" spans="4:22" x14ac:dyDescent="0.25">
@@ -33163,7 +33163,7 @@
       <c r="T810" s="9"/>
       <c r="U810" s="9"/>
       <c r="V810" s="59" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="811" spans="4:22" x14ac:dyDescent="0.25">
@@ -33295,7 +33295,7 @@
       <c r="T814" s="9"/>
       <c r="U814" s="9"/>
       <c r="V814" s="69" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="815" spans="4:22" x14ac:dyDescent="0.25">
@@ -33393,7 +33393,7 @@
       <c r="T817" s="9"/>
       <c r="U817" s="9"/>
       <c r="V817" s="59" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="818" spans="9:22" x14ac:dyDescent="0.25">
@@ -33625,7 +33625,7 @@
       <c r="T824" s="9"/>
       <c r="U824" s="9"/>
       <c r="V824" s="59" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="825" spans="9:22" x14ac:dyDescent="0.25">
@@ -33725,7 +33725,7 @@
       <c r="T827" s="9"/>
       <c r="U827" s="9"/>
       <c r="V827" s="59" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="828" spans="9:22" x14ac:dyDescent="0.25">
@@ -33791,7 +33791,7 @@
       <c r="T829" s="9"/>
       <c r="U829" s="9"/>
       <c r="V829" s="59" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="830" spans="9:22" x14ac:dyDescent="0.25">
@@ -33857,7 +33857,7 @@
       <c r="T831" s="9"/>
       <c r="U831" s="9"/>
       <c r="V831" s="59" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="832" spans="9:22" x14ac:dyDescent="0.25">
@@ -33923,7 +33923,7 @@
       <c r="T833" s="9"/>
       <c r="U833" s="9"/>
       <c r="V833" s="59" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="834" spans="4:22" x14ac:dyDescent="0.25">
@@ -34055,7 +34055,7 @@
       <c r="T837" s="9"/>
       <c r="U837" s="9"/>
       <c r="V837" s="59" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="838" spans="4:22" x14ac:dyDescent="0.25">
@@ -34089,7 +34089,7 @@
       <c r="T838" s="9"/>
       <c r="U838" s="9"/>
       <c r="V838" s="59" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="839" spans="4:22" x14ac:dyDescent="0.25">
@@ -34123,7 +34123,7 @@
       <c r="T839" s="9"/>
       <c r="U839" s="9"/>
       <c r="V839" s="59" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="840" spans="4:22" x14ac:dyDescent="0.25">
@@ -34221,7 +34221,7 @@
       <c r="T842" s="9"/>
       <c r="U842" s="9"/>
       <c r="V842" s="59" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="843" spans="4:22" x14ac:dyDescent="0.25">
@@ -34289,7 +34289,7 @@
       <c r="T844" s="9"/>
       <c r="U844" s="9"/>
       <c r="V844" s="59" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="845" spans="4:22" x14ac:dyDescent="0.25">
@@ -34358,7 +34358,7 @@
       <c r="T846" s="9"/>
       <c r="U846" s="9"/>
       <c r="V846" s="59" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="847" spans="4:22" x14ac:dyDescent="0.25">
@@ -34437,7 +34437,7 @@
         <v>55</v>
       </c>
       <c r="V848" s="59" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="849" spans="8:22" x14ac:dyDescent="0.25">
@@ -34736,7 +34736,7 @@
       <c r="T857" s="9"/>
       <c r="U857" s="9"/>
       <c r="V857" s="59" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="858" spans="8:22" x14ac:dyDescent="0.25">
@@ -34866,7 +34866,7 @@
       <c r="T861" s="9"/>
       <c r="U861" s="9"/>
       <c r="V861" s="59" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="862" spans="8:22" x14ac:dyDescent="0.25">
@@ -35060,7 +35060,7 @@
       <c r="T867" s="9"/>
       <c r="U867" s="9"/>
       <c r="V867" s="59" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="868" spans="4:22" x14ac:dyDescent="0.25">
@@ -35192,7 +35192,7 @@
       <c r="T871" s="9"/>
       <c r="U871" s="9"/>
       <c r="V871" s="59" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="872" spans="4:22" x14ac:dyDescent="0.25">
@@ -35331,7 +35331,7 @@
       </c>
       <c r="U875" s="9"/>
       <c r="V875" s="59" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="876" spans="4:22" x14ac:dyDescent="0.25">
@@ -35625,7 +35625,7 @@
       <c r="T884" s="9"/>
       <c r="U884" s="9"/>
       <c r="V884" s="59" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="885" spans="9:22" x14ac:dyDescent="0.25">
@@ -36319,7 +36319,7 @@
       <c r="T905" s="9"/>
       <c r="U905" s="9"/>
       <c r="V905" s="59" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="906" spans="4:22" x14ac:dyDescent="0.25">
@@ -36873,7 +36873,7 @@
       <c r="T921" s="9"/>
       <c r="U921" s="9"/>
       <c r="V921" s="59" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="922" spans="8:22" x14ac:dyDescent="0.25">
@@ -36939,7 +36939,7 @@
       <c r="T923" s="9"/>
       <c r="U923" s="9"/>
       <c r="V923" s="59" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="924" spans="8:22" x14ac:dyDescent="0.25">
@@ -37005,7 +37005,7 @@
       <c r="T925" s="9"/>
       <c r="U925" s="9"/>
       <c r="V925" s="59" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="926" spans="8:22" x14ac:dyDescent="0.25">
@@ -37683,7 +37683,7 @@
       <c r="T946" s="9"/>
       <c r="U946" s="9"/>
       <c r="V946" s="59" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="947" spans="9:22" x14ac:dyDescent="0.25">
@@ -37749,7 +37749,7 @@
       <c r="T948" s="9"/>
       <c r="U948" s="9"/>
       <c r="V948" s="59" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="949" spans="9:22" x14ac:dyDescent="0.25">
@@ -38007,7 +38007,7 @@
       <c r="T956" s="9"/>
       <c r="U956" s="9"/>
       <c r="V956" s="59" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="957" spans="9:22" x14ac:dyDescent="0.25">
@@ -38073,7 +38073,7 @@
       <c r="T958" s="9"/>
       <c r="U958" s="9"/>
       <c r="V958" s="59" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="959" spans="9:22" x14ac:dyDescent="0.25">
@@ -38107,7 +38107,7 @@
       <c r="T959" s="9"/>
       <c r="U959" s="9"/>
       <c r="V959" s="59" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="960" spans="9:22" x14ac:dyDescent="0.25">
@@ -38204,7 +38204,7 @@
       <c r="T962" s="9"/>
       <c r="U962" s="9"/>
       <c r="V962" s="59" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="963" spans="9:22" x14ac:dyDescent="0.25">
@@ -38558,7 +38558,7 @@
       <c r="T973" s="9"/>
       <c r="U973" s="9"/>
       <c r="V973" s="59" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="974" spans="9:22" x14ac:dyDescent="0.25">
@@ -38848,7 +38848,7 @@
       <c r="T982" s="9"/>
       <c r="U982" s="9"/>
       <c r="V982" s="59" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="983" spans="8:22" x14ac:dyDescent="0.25">
@@ -38882,7 +38882,7 @@
       <c r="T983" s="9"/>
       <c r="U983" s="9"/>
       <c r="V983" s="59" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="984" spans="8:22" x14ac:dyDescent="0.25">
@@ -38989,7 +38989,7 @@
       <c r="T986" s="9"/>
       <c r="U986" s="9"/>
       <c r="V986" s="59" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="987" spans="8:22" x14ac:dyDescent="0.25">
@@ -39221,7 +39221,7 @@
       <c r="T993" s="9"/>
       <c r="U993" s="9"/>
       <c r="V993" s="59" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="994" spans="4:22" x14ac:dyDescent="0.25">
@@ -39319,7 +39319,7 @@
       <c r="T996" s="9"/>
       <c r="U996" s="9"/>
       <c r="V996" s="59" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="997" spans="4:22" x14ac:dyDescent="0.25">
@@ -39373,7 +39373,7 @@
         <v>39</v>
       </c>
       <c r="N998" s="62" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="O998" s="8"/>
       <c r="P998" s="9"/>
@@ -39449,7 +39449,7 @@
       <c r="T1000" s="9"/>
       <c r="U1000" s="9"/>
       <c r="V1000" s="59" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1001" spans="4:22" x14ac:dyDescent="0.25">
@@ -39594,7 +39594,7 @@
       <c r="T1004" s="9"/>
       <c r="U1004" s="9"/>
       <c r="V1004" s="59" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1005" spans="4:22" x14ac:dyDescent="0.25">
@@ -39886,7 +39886,7 @@
       <c r="T1012" s="9"/>
       <c r="U1012" s="9"/>
       <c r="V1012" s="59" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1013" spans="4:22" x14ac:dyDescent="0.25">
@@ -40003,7 +40003,7 @@
       <c r="T1015" s="9"/>
       <c r="U1015" s="9"/>
       <c r="V1015" s="59" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="1016" spans="4:22" x14ac:dyDescent="0.25">
@@ -40069,7 +40069,7 @@
       <c r="T1017" s="9"/>
       <c r="U1017" s="9"/>
       <c r="V1017" s="59" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="1018" spans="4:22" x14ac:dyDescent="0.25">
@@ -40280,7 +40280,7 @@
       <c r="T1023" s="9"/>
       <c r="U1023" s="9"/>
       <c r="V1023" s="59" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1024" spans="4:22" x14ac:dyDescent="0.25">
@@ -40589,7 +40589,7 @@
       <c r="T1032" s="9"/>
       <c r="U1032" s="9"/>
       <c r="V1032" s="59" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="1033" spans="8:22" x14ac:dyDescent="0.25">
@@ -40623,7 +40623,7 @@
       <c r="T1033" s="9"/>
       <c r="U1033" s="9"/>
       <c r="V1033" s="69" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1034" spans="8:22" x14ac:dyDescent="0.25">
@@ -40721,7 +40721,7 @@
       <c r="T1036" s="9"/>
       <c r="U1036" s="9"/>
       <c r="V1036" s="59" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1037" spans="8:22" x14ac:dyDescent="0.25">
@@ -40963,7 +40963,7 @@
       <c r="T1043" s="9"/>
       <c r="U1043" s="9"/>
       <c r="V1043" s="59" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="1044" spans="8:22" x14ac:dyDescent="0.25">
@@ -41221,7 +41221,7 @@
       <c r="T1051" s="9"/>
       <c r="U1051" s="9"/>
       <c r="V1051" s="59" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="1052" spans="8:22" x14ac:dyDescent="0.25">
@@ -41607,7 +41607,7 @@
       <c r="T1063" s="9"/>
       <c r="U1063" s="9"/>
       <c r="V1063" s="59" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="1064" spans="9:22" x14ac:dyDescent="0.25">
@@ -41705,7 +41705,7 @@
       <c r="T1066" s="9"/>
       <c r="U1066" s="9"/>
       <c r="V1066" s="59" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1067" spans="9:22" x14ac:dyDescent="0.25">
@@ -41967,7 +41967,7 @@
       <c r="T1074" s="9"/>
       <c r="U1074" s="9"/>
       <c r="V1074" s="59" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1075" spans="4:22" x14ac:dyDescent="0.25">
@@ -42233,7 +42233,7 @@
       <c r="T1082" s="9"/>
       <c r="U1082" s="9"/>
       <c r="V1082" s="59" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1083" spans="4:22" x14ac:dyDescent="0.25">
@@ -42519,7 +42519,7 @@
       <c r="T1090" s="9"/>
       <c r="U1090" s="9"/>
       <c r="V1090" s="59" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1091" spans="8:22" x14ac:dyDescent="0.25">
@@ -42795,7 +42795,7 @@
         <v>56</v>
       </c>
       <c r="V1098" s="59" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1099" spans="8:22" x14ac:dyDescent="0.25">
@@ -43247,7 +43247,7 @@
       <c r="T1111" s="9"/>
       <c r="U1111" s="9"/>
       <c r="V1111" s="59" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1112" spans="8:22" x14ac:dyDescent="0.25">
@@ -43539,7 +43539,7 @@
       <c r="T1120" s="9"/>
       <c r="U1120" s="9"/>
       <c r="V1120" s="59" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1121" spans="2:22" x14ac:dyDescent="0.25">
@@ -43648,7 +43648,7 @@
       <c r="T1123" s="9"/>
       <c r="U1123" s="9"/>
       <c r="V1123" s="59" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1124" spans="2:22" x14ac:dyDescent="0.25">
@@ -43749,7 +43749,7 @@
       <c r="T1126" s="9"/>
       <c r="U1126" s="9"/>
       <c r="V1126" s="59" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1127" spans="2:22" x14ac:dyDescent="0.25">
@@ -43783,7 +43783,7 @@
       <c r="T1127" s="9"/>
       <c r="U1127" s="9"/>
       <c r="V1127" s="59" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1128" spans="2:22" x14ac:dyDescent="0.25">
@@ -44012,7 +44012,7 @@
       <c r="T1134" s="9"/>
       <c r="U1134" s="9"/>
       <c r="V1134" s="59" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1135" spans="2:22" x14ac:dyDescent="0.25">
@@ -44121,7 +44121,7 @@
       <c r="T1137" s="9"/>
       <c r="U1137" s="9"/>
       <c r="V1137" s="59" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1138" spans="8:22" x14ac:dyDescent="0.25">
@@ -44384,7 +44384,7 @@
       <c r="T1145" s="9"/>
       <c r="U1145" s="9"/>
       <c r="V1145" s="59" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1146" spans="8:22" x14ac:dyDescent="0.25">
@@ -44481,7 +44481,7 @@
       <c r="T1148" s="9"/>
       <c r="U1148" s="9"/>
       <c r="V1148" s="59" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1149" spans="8:22" x14ac:dyDescent="0.25">
@@ -44518,7 +44518,7 @@
       <c r="T1149" s="9"/>
       <c r="U1149" s="9"/>
       <c r="V1149" s="59" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1150" spans="8:22" x14ac:dyDescent="0.25">
@@ -44592,7 +44592,7 @@
       <c r="T1151" s="9"/>
       <c r="U1151" s="9"/>
       <c r="V1151" s="59" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1152" spans="8:22" x14ac:dyDescent="0.25">
@@ -44783,7 +44783,7 @@
       <c r="T1156" s="9"/>
       <c r="U1156" s="9"/>
       <c r="V1156" s="59" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1157" spans="4:22" x14ac:dyDescent="0.25">
@@ -44868,7 +44868,7 @@
       </c>
       <c r="U1158" s="9"/>
       <c r="V1158" s="59" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1159" spans="4:22" x14ac:dyDescent="0.25">
@@ -44902,7 +44902,7 @@
       <c r="T1159" s="9"/>
       <c r="U1159" s="9"/>
       <c r="V1159" s="59" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1160" spans="4:22" x14ac:dyDescent="0.25">
@@ -44968,7 +44968,7 @@
       <c r="T1161" s="9"/>
       <c r="U1161" s="9"/>
       <c r="V1161" s="59" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1162" spans="4:22" x14ac:dyDescent="0.25">
@@ -45098,7 +45098,7 @@
       <c r="T1165" s="9"/>
       <c r="U1165" s="9"/>
       <c r="V1165" s="59" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1166" spans="4:22" x14ac:dyDescent="0.25">
@@ -45206,7 +45206,7 @@
       <c r="T1168" s="9"/>
       <c r="U1168" s="9"/>
       <c r="V1168" s="59" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1169" spans="2:22" x14ac:dyDescent="0.25">
@@ -45341,7 +45341,7 @@
       <c r="T1172" s="9"/>
       <c r="U1172" s="9"/>
       <c r="V1172" s="59" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1173" spans="2:22" x14ac:dyDescent="0.25">
@@ -45375,7 +45375,7 @@
       <c r="T1173" s="9"/>
       <c r="U1173" s="9"/>
       <c r="V1173" s="59" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1174" spans="2:22" x14ac:dyDescent="0.25">
@@ -45665,7 +45665,7 @@
       <c r="T1182" s="9"/>
       <c r="U1182" s="9"/>
       <c r="V1182" s="59" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1183" spans="2:22" x14ac:dyDescent="0.25">
@@ -45699,7 +45699,7 @@
       <c r="T1183" s="9"/>
       <c r="U1183" s="9"/>
       <c r="V1183" s="59" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="1184" spans="2:22" x14ac:dyDescent="0.25">
@@ -46287,7 +46287,7 @@
       <c r="T1201" s="9"/>
       <c r="U1201" s="9"/>
       <c r="V1201" s="59" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="1202" spans="9:22" x14ac:dyDescent="0.25">
@@ -46321,7 +46321,7 @@
       <c r="T1202" s="9"/>
       <c r="U1202" s="9"/>
       <c r="V1202" s="59" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1203" spans="9:22" x14ac:dyDescent="0.25">
@@ -46515,7 +46515,7 @@
       <c r="T1208" s="9"/>
       <c r="U1208" s="9"/>
       <c r="V1208" s="69" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1209" spans="9:22" x14ac:dyDescent="0.25">
@@ -46805,7 +46805,7 @@
       <c r="T1217" s="9"/>
       <c r="U1217" s="9"/>
       <c r="V1217" s="59" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1218" spans="8:22" x14ac:dyDescent="0.25">
@@ -46839,7 +46839,7 @@
       <c r="T1218" s="9"/>
       <c r="U1218" s="9"/>
       <c r="V1218" s="59" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1219" spans="8:22" x14ac:dyDescent="0.25">
@@ -46937,7 +46937,7 @@
       <c r="T1221" s="9"/>
       <c r="U1221" s="9"/>
       <c r="V1221" s="59" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1222" spans="8:22" x14ac:dyDescent="0.25">
@@ -46971,7 +46971,7 @@
       <c r="T1222" s="9"/>
       <c r="U1222" s="9"/>
       <c r="V1222" s="59" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1223" spans="8:22" x14ac:dyDescent="0.25">
@@ -47342,7 +47342,7 @@
       <c r="T1233" s="9"/>
       <c r="U1233" s="9"/>
       <c r="V1233" s="59" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1234" spans="8:22" x14ac:dyDescent="0.25">
@@ -47540,7 +47540,7 @@
       <c r="T1239" s="9"/>
       <c r="U1239" s="9"/>
       <c r="V1239" s="59" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1240" spans="8:22" x14ac:dyDescent="0.25">
@@ -47670,7 +47670,7 @@
       <c r="T1243" s="9"/>
       <c r="U1243" s="9"/>
       <c r="V1243" s="59" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1244" spans="8:22" x14ac:dyDescent="0.25">
@@ -47704,7 +47704,7 @@
       <c r="T1244" s="9"/>
       <c r="U1244" s="9"/>
       <c r="V1244" s="59" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1245" spans="8:22" x14ac:dyDescent="0.25">
@@ -47964,7 +47964,7 @@
       <c r="T1252" s="9"/>
       <c r="U1252" s="9"/>
       <c r="V1252" s="59" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1253" spans="9:22" x14ac:dyDescent="0.25">
@@ -48158,7 +48158,7 @@
       <c r="T1258" s="9"/>
       <c r="U1258" s="9"/>
       <c r="V1258" s="59" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1259" spans="9:22" x14ac:dyDescent="0.25">
@@ -48288,7 +48288,7 @@
       <c r="T1262" s="9"/>
       <c r="U1262" s="9"/>
       <c r="V1262" s="59" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1263" spans="9:22" x14ac:dyDescent="0.25">
@@ -48557,7 +48557,7 @@
         <v>62</v>
       </c>
       <c r="V1270" s="59" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1271" spans="5:22" x14ac:dyDescent="0.25">
@@ -48599,7 +48599,7 @@
         <v>56</v>
       </c>
       <c r="V1271" s="69" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1272" spans="5:22" x14ac:dyDescent="0.25">
@@ -48793,7 +48793,7 @@
       <c r="T1277" s="9"/>
       <c r="U1277" s="9"/>
       <c r="V1277" s="59" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1278" spans="5:22" x14ac:dyDescent="0.25">
@@ -48859,7 +48859,7 @@
       <c r="T1279" s="9"/>
       <c r="U1279" s="9"/>
       <c r="V1279" s="59" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1280" spans="5:22" x14ac:dyDescent="0.25">
@@ -48925,7 +48925,7 @@
       <c r="T1281" s="9"/>
       <c r="U1281" s="9"/>
       <c r="V1281" s="59" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1282" spans="9:22" x14ac:dyDescent="0.25">
@@ -48991,7 +48991,7 @@
       <c r="T1283" s="9"/>
       <c r="U1283" s="9"/>
       <c r="V1283" s="59" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1284" spans="9:22" x14ac:dyDescent="0.25">
@@ -49153,7 +49153,7 @@
       <c r="T1288" s="9"/>
       <c r="U1288" s="9"/>
       <c r="V1288" s="59" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="1289" spans="9:22" x14ac:dyDescent="0.25">
@@ -49283,7 +49283,7 @@
       <c r="T1292" s="9"/>
       <c r="U1292" s="9"/>
       <c r="V1292" s="59" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1293" spans="9:22" x14ac:dyDescent="0.25">
@@ -49801,7 +49801,7 @@
       <c r="T1308" s="9"/>
       <c r="U1308" s="9"/>
       <c r="V1308" s="59" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1309" spans="3:22" x14ac:dyDescent="0.25">
@@ -49913,7 +49913,7 @@
         <v>3</v>
       </c>
       <c r="N1311" s="76" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="O1311" s="9" t="s">
         <v>49</v>
@@ -49925,7 +49925,7 @@
       <c r="T1311" s="9"/>
       <c r="U1311" s="9"/>
       <c r="V1311" s="59" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1312" spans="3:22" x14ac:dyDescent="0.25">
@@ -50102,7 +50102,7 @@
       <c r="T1316" s="9"/>
       <c r="U1316" s="9"/>
       <c r="V1316" s="59" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1317" spans="3:22" x14ac:dyDescent="0.25">
@@ -50419,7 +50419,7 @@
       <c r="T1325" s="9"/>
       <c r="U1325" s="9"/>
       <c r="V1325" s="59" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1326" spans="3:22" x14ac:dyDescent="0.25">
@@ -50535,7 +50535,7 @@
       <c r="T1328" s="9"/>
       <c r="U1328" s="9"/>
       <c r="V1328" s="59" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1329" spans="3:22" x14ac:dyDescent="0.25">
@@ -50613,7 +50613,7 @@
       <c r="T1330" s="9"/>
       <c r="U1330" s="9"/>
       <c r="V1330" s="59" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1331" spans="3:22" x14ac:dyDescent="0.25">
@@ -50767,7 +50767,7 @@
       <c r="S1334" s="9"/>
       <c r="T1334" s="9"/>
       <c r="V1334" s="75" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1335" spans="3:22" x14ac:dyDescent="0.25">
@@ -50875,7 +50875,7 @@
       <c r="T1337" s="9"/>
       <c r="U1337" s="9"/>
       <c r="V1337" s="59" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="1338" spans="3:22" x14ac:dyDescent="0.25">
@@ -50912,7 +50912,7 @@
       <c r="T1338" s="9"/>
       <c r="U1338" s="9"/>
       <c r="V1338" s="59" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1339" spans="3:22" x14ac:dyDescent="0.25">
@@ -50949,7 +50949,7 @@
       <c r="T1339" s="9"/>
       <c r="U1339" s="9"/>
       <c r="V1339" s="59" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1340" spans="3:22" x14ac:dyDescent="0.25">
@@ -51056,7 +51056,7 @@
       <c r="T1342" s="9"/>
       <c r="U1342" s="9"/>
       <c r="V1342" s="59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1343" spans="3:22" x14ac:dyDescent="0.25">
@@ -51093,7 +51093,7 @@
       <c r="T1343" s="9"/>
       <c r="U1343" s="9"/>
       <c r="V1343" s="59" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1344" spans="3:22" x14ac:dyDescent="0.25">
@@ -51200,7 +51200,7 @@
       <c r="T1346" s="9"/>
       <c r="U1346" s="9"/>
       <c r="V1346" s="59" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1347" spans="3:22" x14ac:dyDescent="0.25">
@@ -51237,7 +51237,7 @@
       <c r="T1347" s="9"/>
       <c r="U1347" s="9"/>
       <c r="V1347" s="59" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1348" spans="3:22" x14ac:dyDescent="0.25">
@@ -51344,7 +51344,7 @@
       <c r="T1350" s="9"/>
       <c r="U1350" s="9"/>
       <c r="V1350" s="59" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1351" spans="3:22" x14ac:dyDescent="0.25">
@@ -51486,7 +51486,7 @@
       <c r="T1354" s="9"/>
       <c r="U1354" s="9"/>
       <c r="V1354" s="59" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1355" spans="3:22" x14ac:dyDescent="0.25">
@@ -51558,7 +51558,7 @@
       <c r="T1356" s="9"/>
       <c r="U1356" s="9"/>
       <c r="V1356" s="59" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1357" spans="3:22" x14ac:dyDescent="0.25">
@@ -51595,7 +51595,7 @@
       <c r="T1357" s="9"/>
       <c r="U1357" s="9"/>
       <c r="V1357" s="59" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1358" spans="3:22" x14ac:dyDescent="0.25">
@@ -51632,7 +51632,7 @@
       <c r="T1358" s="9"/>
       <c r="U1358" s="9"/>
       <c r="V1358" s="59" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1359" spans="3:22" x14ac:dyDescent="0.25">
@@ -51786,7 +51786,7 @@
       <c r="T1362" s="9"/>
       <c r="U1362" s="9"/>
       <c r="V1362" s="59" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1363" spans="3:22" x14ac:dyDescent="0.25">
@@ -52001,7 +52001,7 @@
       <c r="T1368" s="9"/>
       <c r="U1368" s="9"/>
       <c r="V1368" s="59" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1369" spans="3:22" x14ac:dyDescent="0.25">
@@ -52316,7 +52316,7 @@
       <c r="T1376" s="9"/>
       <c r="U1376" s="9"/>
       <c r="V1376" s="59" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1377" spans="3:22" x14ac:dyDescent="0.25">
@@ -52423,7 +52423,7 @@
       <c r="T1379" s="9"/>
       <c r="U1379" s="9"/>
       <c r="V1379" s="59" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1380" spans="3:22" x14ac:dyDescent="0.25">
@@ -52463,7 +52463,7 @@
       <c r="T1380" s="9"/>
       <c r="U1380" s="9"/>
       <c r="V1380" s="59" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1381" spans="3:22" x14ac:dyDescent="0.25">
@@ -52503,7 +52503,7 @@
       <c r="T1381" s="9"/>
       <c r="U1381" s="9"/>
       <c r="V1381" s="59" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1382" spans="3:22" x14ac:dyDescent="0.25">
@@ -52728,7 +52728,7 @@
       <c r="T1387" s="9"/>
       <c r="U1387" s="9"/>
       <c r="V1387" s="59" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1388" spans="3:22" x14ac:dyDescent="0.25">
@@ -52905,7 +52905,7 @@
       <c r="T1392" s="9"/>
       <c r="U1392" s="9"/>
       <c r="V1392" s="59" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1393" spans="3:22" x14ac:dyDescent="0.25">
@@ -52942,7 +52942,7 @@
       <c r="T1393" s="9"/>
       <c r="U1393" s="9"/>
       <c r="V1393" s="59" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1394" spans="3:22" x14ac:dyDescent="0.25">
@@ -53051,7 +53051,7 @@
       <c r="T1396" s="9"/>
       <c r="U1396" s="9"/>
       <c r="V1396" s="59" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1397" spans="3:22" x14ac:dyDescent="0.25">
@@ -53263,7 +53263,7 @@
       <c r="T1402" s="9"/>
       <c r="U1402" s="9"/>
       <c r="V1402" s="59" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1403" spans="3:22" x14ac:dyDescent="0.25">
@@ -53565,7 +53565,7 @@
       <c r="T1410" s="9"/>
       <c r="U1410" s="9"/>
       <c r="V1410" s="59" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1411" spans="3:22" x14ac:dyDescent="0.25">
@@ -53672,7 +53672,7 @@
       <c r="T1413" s="9"/>
       <c r="U1413" s="9"/>
       <c r="V1413" s="59" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1414" spans="3:22" x14ac:dyDescent="0.25">
@@ -53886,7 +53886,7 @@
       <c r="T1419" s="9"/>
       <c r="U1419" s="9"/>
       <c r="V1419" s="59" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1420" spans="3:22" x14ac:dyDescent="0.25">
@@ -53923,7 +53923,7 @@
       <c r="T1420" s="9"/>
       <c r="U1420" s="9"/>
       <c r="V1420" s="59" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1421" spans="3:22" x14ac:dyDescent="0.25">
@@ -54030,7 +54030,7 @@
       <c r="T1423" s="9"/>
       <c r="U1423" s="9"/>
       <c r="V1423" s="59" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1424" spans="3:22" x14ac:dyDescent="0.25">
@@ -54172,7 +54172,7 @@
       <c r="T1427" s="9"/>
       <c r="U1427" s="9"/>
       <c r="V1427" s="59" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1428" spans="2:22" x14ac:dyDescent="0.25">
@@ -54279,7 +54279,7 @@
       <c r="T1430" s="9"/>
       <c r="U1430" s="9"/>
       <c r="V1430" s="59" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1431" spans="2:22" x14ac:dyDescent="0.25">
@@ -54499,7 +54499,7 @@
       <c r="T1436" s="9"/>
       <c r="U1436" s="9"/>
       <c r="V1436" s="59" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1437" spans="2:22" x14ac:dyDescent="0.25">
@@ -54746,7 +54746,7 @@
       <c r="T1443" s="9"/>
       <c r="U1443" s="9"/>
       <c r="V1443" s="59" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1444" spans="2:22" x14ac:dyDescent="0.25">
@@ -54783,7 +54783,7 @@
       <c r="T1444" s="9"/>
       <c r="U1444" s="9"/>
       <c r="V1444" s="59" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1445" spans="2:22" x14ac:dyDescent="0.25">
@@ -55143,7 +55143,7 @@
       <c r="T1454" s="9"/>
       <c r="U1454" s="9"/>
       <c r="V1454" s="59" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1455" spans="2:22" x14ac:dyDescent="0.25">
@@ -55641,7 +55641,7 @@
       <c r="T1467" s="9"/>
       <c r="U1467" s="9"/>
       <c r="V1467" s="59" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1468" spans="3:22" x14ac:dyDescent="0.25">
@@ -55894,7 +55894,7 @@
       <c r="T1474" s="9"/>
       <c r="U1474" s="9"/>
       <c r="V1474" s="59" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1475" spans="3:22" x14ac:dyDescent="0.25">
@@ -56196,7 +56196,7 @@
       <c r="T1482" s="9"/>
       <c r="U1482" s="9"/>
       <c r="V1482" s="59" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1483" spans="3:22" x14ac:dyDescent="0.25">
@@ -56419,7 +56419,7 @@
       <c r="T1488" s="9"/>
       <c r="U1488" s="9"/>
       <c r="V1488" s="59" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1489" spans="2:22" x14ac:dyDescent="0.25">
@@ -56493,7 +56493,7 @@
       <c r="T1490" s="9"/>
       <c r="U1490" s="9"/>
       <c r="V1490" s="59" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1491" spans="2:22" x14ac:dyDescent="0.25">
@@ -56530,7 +56530,7 @@
       <c r="T1491" s="9"/>
       <c r="U1491" s="9"/>
       <c r="V1491" s="59" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1492" spans="2:22" x14ac:dyDescent="0.25">
@@ -56921,7 +56921,7 @@
       <c r="T1502" s="9"/>
       <c r="U1502" s="9"/>
       <c r="V1502" s="59" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1503" spans="2:22" x14ac:dyDescent="0.25">
@@ -57036,7 +57036,7 @@
       <c r="T1505" s="9"/>
       <c r="U1505" s="9"/>
       <c r="V1505" s="59" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1506" spans="3:22" x14ac:dyDescent="0.25">
@@ -57217,7 +57217,7 @@
       <c r="T1510" s="9"/>
       <c r="U1510" s="9"/>
       <c r="V1510" s="59" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1511" spans="3:22" x14ac:dyDescent="0.25">
@@ -57324,7 +57324,7 @@
       <c r="T1513" s="9"/>
       <c r="U1513" s="9"/>
       <c r="V1513" s="59" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1514" spans="3:22" x14ac:dyDescent="0.25">
@@ -57476,7 +57476,7 @@
       <c r="T1517" s="9"/>
       <c r="U1517" s="9"/>
       <c r="V1517" s="59" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1518" spans="3:22" x14ac:dyDescent="0.25">
@@ -57622,7 +57622,7 @@
         <v>56</v>
       </c>
       <c r="V1521" s="59" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1522" spans="2:22" x14ac:dyDescent="0.25">
@@ -57958,7 +57958,7 @@
       <c r="T1530" s="9"/>
       <c r="U1530" s="9"/>
       <c r="V1530" s="59" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1531" spans="2:22" x14ac:dyDescent="0.25">
@@ -57995,7 +57995,7 @@
       <c r="T1531" s="9"/>
       <c r="U1531" s="9"/>
       <c r="V1531" s="59" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1532" spans="2:22" x14ac:dyDescent="0.25">

</xml_diff>